<commit_message>
feta: generating the graphs
</commit_message>
<xml_diff>
--- a/predictions/prediction-charts-500-curso-sagemaker-canvas-dio.xlsx
+++ b/predictions/prediction-charts-500-curso-sagemaker-canvas-dio.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/84f914e38f2c05d3/Documentos/Dio Cursos Bootcamps/Nexa Machine Learning e GenAI na Pratica/dio-lab-aws-sagemaker-canvas-estoque/predictions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{FF000658-05ED-44FC-9043-A0B289B64807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDC2F564-FAEF-456F-A637-A7E080D5BB67}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="8_{FF000658-05ED-44FC-9043-A0B289B64807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5F1FC2B-F9A2-45FA-A281-6629DF4EF76A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{508E80D1-B4AE-4F8C-8854-F6EC913DBE24}"/>
   </bookViews>
   <sheets>
     <sheet name="prediction-charts-500-curso-sag" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -42,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>ID_PRODUTO</t>
   </si>
@@ -97,13 +110,28 @@
   <si>
     <t>Faixa Inferior (P10)</t>
   </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>P50</t>
+  </si>
+  <si>
+    <t>P90</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Faixa De Incerteza (P90 - P10)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -585,7 +613,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -659,6 +687,32 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Percentis de Previsão de Estoque por Produto (Ordenado por Risco de Ruptura)</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -703,7 +757,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p10</c:v>
+                  <c:v>P10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -711,7 +765,10 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -916,7 +973,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p50</c:v>
+                  <c:v>P50</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1129,7 +1186,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p90</c:v>
+                  <c:v>P90</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1137,7 +1194,10 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1353,10 +1413,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" b="1"/>
+                  <a:t>ID do Produto (ordenado por P10 crescente)</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1392,7 +1508,7 @@
         </c:txPr>
         <c:crossAx val="1479463120"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
+        <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
@@ -1418,14 +1534,49 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1450,7 +1601,1785 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1479466000"/>
+        <c:crossesAt val="1"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Faixa de Incerteza da Previsão de Estoque por Produto </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>(Ordenada por Risco de Ruptura)</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'prediction-charts-500-curso-sag'!$H$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Faixa Inferior (P10)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'prediction-charts-500-curso-sag'!$A$29:$A$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'prediction-charts-500-curso-sag'!$H$29:$H$53</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>-26.288927659999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-25.557365359999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-25.397923800000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-22.913674530000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-22.644954899999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-22.092060190000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-20.606256309999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-19.471835949999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-17.60299328</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-17.309159149999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-16.841649100000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-16.792418179999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-15.893228560000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-15.52131189</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-11.33110662</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-10.14274846</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-9.6547029339999995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-5.229760035</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-5.08711994</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-3.5482118310000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.1854626847143299</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11.870232430570899</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>17.321052095945699</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>19.872057633683401</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24.705846500042099</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4BAB-42EA-A885-D223B5EEF32A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'prediction-charts-500-curso-sag'!$I$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Faixa De Incerteza (P90 - P10)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'prediction-charts-500-curso-sag'!$A$29:$A$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'prediction-charts-500-curso-sag'!$I$29:$I$53</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>14.593316269999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.2072670199999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.8976694000000016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.596966364000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.438279789999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.071527810000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.879237718999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.8418843299999992</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.970648805</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.6588620219999992</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.1767717390000012</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.9308516049999991</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.3243073110000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.4022407210000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.3719557689999995</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.9251547020000004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.3975614929999995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.5738880330000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.3656185220000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.1891926390000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.1215655159365694</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.6001381133172021</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.1305252029240016</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.2853406495058977</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.1550975078076</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-4BAB-42EA-A885-D223B5EEF32A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1479466000"/>
+        <c:axId val="1479463120"/>
+      </c:areaChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'prediction-charts-500-curso-sag'!$D$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'prediction-charts-500-curso-sag'!$A$29:$A$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'prediction-charts-500-curso-sag'!$D$29:$D$53</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>-17.811083</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-21.183490859999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-20.234597860000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-16.12091015</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-15.636835700000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-17.558217280000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-13.480506849999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-16.209189429999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-11.39064576</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-13.44040889</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-11.717122760000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-13.22168973</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-12.50630321</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-11.78787309</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-9.6277013149999995</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-7.2224097709999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-7.1852992589999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-2.9637752759999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-2.5364973499999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-2.9117336260000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.1917846185586694</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15.396013582861199</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18.9909651615685</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>21.874890344312199</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26.6952477090896</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-4BAB-42EA-A885-D223B5EEF32A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1479466000"/>
+        <c:axId val="1479463120"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1479466000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" b="1"/>
+                  <a:t>ID do Produto (ordenado por P10 crescente)</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1479463120"/>
         <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1479463120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1479466000"/>
+        <c:crossesAt val="1"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:noFill/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12995525691522516"/>
+          <c:y val="0.94159959437097229"/>
+          <c:w val="0.52030043181548502"/>
+          <c:h val="4.2022715490094432E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Comparativo de Estoque Previsto por Produto </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>(Ordenado por Risco de Ruptura)</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'prediction-charts-500-curso-sag'!$D$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'prediction-charts-500-curso-sag'!$K$29:$K$53</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="25"/>
+                  <c:pt idx="0">
+                    <c:v>6.1154716100000002</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.8333925200000003</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.7343434600000016</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7.8042019840000005</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5.4301605899999998</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>5.5376849000000004</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7.7534882589999992</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3.5792378099999986</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>6.7583012849999999</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.7901117620000004</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>4.0522453990000002</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>4.3601231550000001</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>3.9373819609999998</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.668801921</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>1.6685504639999991</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>3.0048160130000001</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>2.9281578179999999</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>2.3079032740000001</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.814995932</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>0.55271443400000031</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>2.11524358209223</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>2.0743569610269024</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>2.4606121373012009</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>1.2825079388770995</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>2.1656962987600998</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'prediction-charts-500-curso-sag'!$L$29:$L$53</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="25"/>
+                  <c:pt idx="0">
+                    <c:v>8.4778446599999988</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.3738744999999994</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5.16332594</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.7927643800000013</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.0081191999999977</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.5338429100000006</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7.1257494599999998</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3.2626465200000005</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>6.2123475199999998</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.8687502599999988</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>5.124526340000001</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>3.5707284499999989</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>3.3869253500000003</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.7334388000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>1.7034053050000004</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>2.9203386890000003</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>2.4694036749999997</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>2.2659847590000002</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>2.5506225900000001</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>0.63647820499999996</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>3.0063219338443394</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>3.5257811522902998</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>1.6699130656228007</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>2.0028327106287982</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>1.9894012090475002</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="22225" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>'prediction-charts-500-curso-sag'!$A$29:$A$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'prediction-charts-500-curso-sag'!$D$29:$D$53</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>-17.811083</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-21.183490859999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-20.234597860000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-16.12091015</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-15.636835700000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-17.558217280000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-13.480506849999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-16.209189429999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-11.39064576</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-13.44040889</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-11.717122760000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-13.22168973</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-12.50630321</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-11.78787309</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-9.6277013149999995</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-7.2224097709999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-7.1852992589999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-2.9637752759999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-2.5364973499999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-2.9117336260000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.1917846185586694</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15.396013582861199</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18.9909651615685</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>21.874890344312199</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26.6952477090896</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A2E7-4B02-A650-BAC7570C6036}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1479466000"/>
+        <c:axId val="1479463120"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1479466000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR" b="1"/>
+                  <a:t>ID do Produto (ordenado por P10 crescente)</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1479463120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1479463120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1479466000"/>
+        <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -1537,6 +3466,86 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2079,20 +4088,1026 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>468085</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>54429</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>14512</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>239485</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>174172</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>377370</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>137885</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2117,7 +5132,87 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>36285</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>399143</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>119742</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05297EDB-8376-4CDA-96AD-F95A923DCC5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>57</xdr:col>
+      <xdr:colOff>362859</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>137885</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39A11D75-44E3-40A7-A8F8-BAD234030F10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2439,8 +5534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B05673-5FEF-4C8E-A9C9-6CE58C9393BC}">
   <dimension ref="A1:M1130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:E53"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="48" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AX36" sqref="AX36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3393,16 +6488,28 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E28" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F28" t="s">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="H28" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" t="s">
+        <v>6</v>
+      </c>
+      <c r="L28" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
@@ -3424,6 +6531,22 @@
       <c r="F29" s="2">
         <v>-18.65310581</v>
       </c>
+      <c r="H29" s="2">
+        <f>C29</f>
+        <v>-26.288927659999999</v>
+      </c>
+      <c r="I29" s="2">
+        <f>E29-C29</f>
+        <v>14.593316269999999</v>
+      </c>
+      <c r="K29" s="2">
+        <f>E29-D29</f>
+        <v>6.1154716100000002</v>
+      </c>
+      <c r="L29" s="2">
+        <f>D29-C29</f>
+        <v>8.4778446599999988</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
@@ -3444,6 +6567,22 @@
       <c r="F30" s="2">
         <v>-21.20098033</v>
       </c>
+      <c r="H30" s="2">
+        <f t="shared" ref="H30:H53" si="4">C30</f>
+        <v>-25.557365359999999</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" ref="I30:I53" si="5">E30-C30</f>
+        <v>9.2072670199999997</v>
+      </c>
+      <c r="K30" s="2">
+        <f t="shared" ref="K30:K53" si="6">E30-D30</f>
+        <v>4.8333925200000003</v>
+      </c>
+      <c r="L30" s="2">
+        <f t="shared" ref="L30:L53" si="7">D30-C30</f>
+        <v>4.3738744999999994</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
@@ -3464,6 +6603,22 @@
       <c r="F31" s="2">
         <v>-20.330828950000001</v>
       </c>
+      <c r="H31" s="2">
+        <f t="shared" si="4"/>
+        <v>-25.397923800000001</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="5"/>
+        <v>9.8976694000000016</v>
+      </c>
+      <c r="K31" s="2">
+        <f t="shared" si="6"/>
+        <v>4.7343434600000016</v>
+      </c>
+      <c r="L31" s="2">
+        <f t="shared" si="7"/>
+        <v>5.16332594</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
@@ -3484,8 +6639,24 @@
       <c r="F32" s="2">
         <v>-15.46039642</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H32" s="2">
+        <f t="shared" si="4"/>
+        <v>-22.913674530000002</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="5"/>
+        <v>14.596966364000002</v>
+      </c>
+      <c r="K32" s="2">
+        <f t="shared" si="6"/>
+        <v>7.8042019840000005</v>
+      </c>
+      <c r="L32" s="2">
+        <f t="shared" si="7"/>
+        <v>6.7927643800000013</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
@@ -3504,8 +6675,24 @@
       <c r="F33" s="2">
         <v>-16.02102588</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H33" s="2">
+        <f t="shared" si="4"/>
+        <v>-22.644954899999998</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="5"/>
+        <v>12.438279789999998</v>
+      </c>
+      <c r="K33" s="2">
+        <f t="shared" si="6"/>
+        <v>5.4301605899999998</v>
+      </c>
+      <c r="L33" s="2">
+        <f t="shared" si="7"/>
+        <v>7.0081191999999977</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>10</v>
       </c>
@@ -3524,8 +6711,24 @@
       <c r="F34" s="2">
         <v>-17.327571720000002</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H34" s="2">
+        <f t="shared" si="4"/>
+        <v>-22.092060190000002</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="5"/>
+        <v>10.071527810000001</v>
+      </c>
+      <c r="K34" s="2">
+        <f t="shared" si="6"/>
+        <v>5.5376849000000004</v>
+      </c>
+      <c r="L34" s="2">
+        <f t="shared" si="7"/>
+        <v>4.5338429100000006</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>11</v>
       </c>
@@ -3544,8 +6747,24 @@
       <c r="F35" s="2">
         <v>-13.42965324</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H35" s="2">
+        <f t="shared" si="4"/>
+        <v>-20.606256309999999</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="5"/>
+        <v>14.879237718999999</v>
+      </c>
+      <c r="K35" s="2">
+        <f t="shared" si="6"/>
+        <v>7.7534882589999992</v>
+      </c>
+      <c r="L35" s="2">
+        <f t="shared" si="7"/>
+        <v>7.1257494599999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>14</v>
       </c>
@@ -3564,8 +6783,24 @@
       <c r="F36" s="2">
         <v>-16.214258109999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H36" s="2">
+        <f t="shared" si="4"/>
+        <v>-19.471835949999999</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="5"/>
+        <v>6.8418843299999992</v>
+      </c>
+      <c r="K36" s="2">
+        <f t="shared" si="6"/>
+        <v>3.5792378099999986</v>
+      </c>
+      <c r="L36" s="2">
+        <f t="shared" si="7"/>
+        <v>3.2626465200000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>6</v>
       </c>
@@ -3584,8 +6819,24 @@
       <c r="F37" s="2">
         <v>-11.47511493</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H37" s="2">
+        <f t="shared" si="4"/>
+        <v>-17.60299328</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="5"/>
+        <v>12.970648805</v>
+      </c>
+      <c r="K37" s="2">
+        <f t="shared" si="6"/>
+        <v>6.7583012849999999</v>
+      </c>
+      <c r="L37" s="2">
+        <f t="shared" si="7"/>
+        <v>6.2123475199999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>25</v>
       </c>
@@ -3604,8 +6855,24 @@
       <c r="F38" s="2">
         <v>-13.410662840000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H38" s="2">
+        <f t="shared" si="4"/>
+        <v>-17.309159149999999</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="5"/>
+        <v>7.6588620219999992</v>
+      </c>
+      <c r="K38" s="2">
+        <f t="shared" si="6"/>
+        <v>3.7901117620000004</v>
+      </c>
+      <c r="L38" s="2">
+        <f t="shared" si="7"/>
+        <v>3.8687502599999988</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>24</v>
       </c>
@@ -3624,8 +6891,24 @@
       <c r="F39" s="2">
         <v>-12.27767674</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H39" s="2">
+        <f t="shared" si="4"/>
+        <v>-16.841649100000001</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="5"/>
+        <v>9.1767717390000012</v>
+      </c>
+      <c r="K39" s="2">
+        <f t="shared" si="6"/>
+        <v>4.0522453990000002</v>
+      </c>
+      <c r="L39" s="2">
+        <f t="shared" si="7"/>
+        <v>5.124526340000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>18</v>
       </c>
@@ -3644,8 +6927,24 @@
       <c r="F40" s="2">
         <v>-13.10857661</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H40" s="2">
+        <f t="shared" si="4"/>
+        <v>-16.792418179999999</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="5"/>
+        <v>7.9308516049999991</v>
+      </c>
+      <c r="K40" s="2">
+        <f t="shared" si="6"/>
+        <v>4.3601231550000001</v>
+      </c>
+      <c r="L40" s="2">
+        <f t="shared" si="7"/>
+        <v>3.5707284499999989</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>19</v>
       </c>
@@ -3664,8 +6963,24 @@
       <c r="F41" s="2">
         <v>-12.305795809999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H41" s="2">
+        <f t="shared" si="4"/>
+        <v>-15.893228560000001</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="5"/>
+        <v>7.3243073110000001</v>
+      </c>
+      <c r="K41" s="2">
+        <f t="shared" si="6"/>
+        <v>3.9373819609999998</v>
+      </c>
+      <c r="L41" s="2">
+        <f t="shared" si="7"/>
+        <v>3.3869253500000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>4</v>
       </c>
@@ -3684,8 +6999,24 @@
       <c r="F42" s="2">
         <v>-11.97825667</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H42" s="2">
+        <f t="shared" si="4"/>
+        <v>-15.52131189</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="5"/>
+        <v>7.4022407210000001</v>
+      </c>
+      <c r="K42" s="2">
+        <f t="shared" si="6"/>
+        <v>3.668801921</v>
+      </c>
+      <c r="L42" s="2">
+        <f t="shared" si="7"/>
+        <v>3.7334388000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>7</v>
       </c>
@@ -3704,8 +7035,24 @@
       <c r="F43" s="2">
         <v>-9.595270953</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H43" s="2">
+        <f t="shared" si="4"/>
+        <v>-11.33110662</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3719557689999995</v>
+      </c>
+      <c r="K43" s="2">
+        <f t="shared" si="6"/>
+        <v>1.6685504639999991</v>
+      </c>
+      <c r="L43" s="2">
+        <f t="shared" si="7"/>
+        <v>1.7034053050000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>8</v>
       </c>
@@ -3724,8 +7071,24 @@
       <c r="F44" s="2">
         <v>-7.0628070730000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H44" s="2">
+        <f t="shared" si="4"/>
+        <v>-10.14274846</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="5"/>
+        <v>5.9251547020000004</v>
+      </c>
+      <c r="K44" s="2">
+        <f t="shared" si="6"/>
+        <v>3.0048160130000001</v>
+      </c>
+      <c r="L44" s="2">
+        <f t="shared" si="7"/>
+        <v>2.9203386890000003</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>20</v>
       </c>
@@ -3744,8 +7107,24 @@
       <c r="F45" s="2">
         <v>-7.1789580199999996</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H45" s="2">
+        <f t="shared" si="4"/>
+        <v>-9.6547029339999995</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="5"/>
+        <v>5.3975614929999995</v>
+      </c>
+      <c r="K45" s="2">
+        <f t="shared" si="6"/>
+        <v>2.9281578179999999</v>
+      </c>
+      <c r="L45" s="2">
+        <f t="shared" si="7"/>
+        <v>2.4694036749999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>9</v>
       </c>
@@ -3764,8 +7143,24 @@
       <c r="F46" s="2">
         <v>-2.960465084</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H46" s="2">
+        <f t="shared" si="4"/>
+        <v>-5.229760035</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="5"/>
+        <v>4.5738880330000002</v>
+      </c>
+      <c r="K46" s="2">
+        <f t="shared" si="6"/>
+        <v>2.3079032740000001</v>
+      </c>
+      <c r="L46" s="2">
+        <f t="shared" si="7"/>
+        <v>2.2659847590000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>17</v>
       </c>
@@ -3784,8 +7179,24 @@
       <c r="F47" s="2">
         <v>-2.8133533489999998</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H47" s="2">
+        <f t="shared" si="4"/>
+        <v>-5.08711994</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="5"/>
+        <v>4.3656185220000001</v>
+      </c>
+      <c r="K47" s="2">
+        <f t="shared" si="6"/>
+        <v>1.814995932</v>
+      </c>
+      <c r="L47" s="2">
+        <f t="shared" si="7"/>
+        <v>2.5506225900000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>23</v>
       </c>
@@ -3803,6 +7214,22 @@
       </c>
       <c r="F48" s="2">
         <v>-2.9407601240000001</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="4"/>
+        <v>-3.5482118310000001</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="5"/>
+        <v>1.1891926390000003</v>
+      </c>
+      <c r="K48" s="2">
+        <f t="shared" si="6"/>
+        <v>0.55271443400000031</v>
+      </c>
+      <c r="L48" s="2">
+        <f t="shared" si="7"/>
+        <v>0.63647820499999996</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
@@ -3824,6 +7251,22 @@
       <c r="F49" s="2">
         <v>7.9972845297301403</v>
       </c>
+      <c r="H49" s="2">
+        <f t="shared" si="4"/>
+        <v>5.1854626847143299</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="5"/>
+        <v>5.1215655159365694</v>
+      </c>
+      <c r="K49" s="2">
+        <f t="shared" si="6"/>
+        <v>2.11524358209223</v>
+      </c>
+      <c r="L49" s="2">
+        <f t="shared" si="7"/>
+        <v>3.0063219338443394</v>
+      </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
@@ -3843,6 +7286,22 @@
       </c>
       <c r="F50" s="2">
         <v>14.905419644526701</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="4"/>
+        <v>11.870232430570899</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="5"/>
+        <v>5.6001381133172021</v>
+      </c>
+      <c r="K50" s="2">
+        <f t="shared" si="6"/>
+        <v>2.0743569610269024</v>
+      </c>
+      <c r="L50" s="2">
+        <f t="shared" si="7"/>
+        <v>3.5257811522902998</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
@@ -3864,6 +7323,22 @@
       <c r="F51" s="2">
         <v>19.180894711916501</v>
       </c>
+      <c r="H51" s="2">
+        <f t="shared" si="4"/>
+        <v>17.321052095945699</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="5"/>
+        <v>4.1305252029240016</v>
+      </c>
+      <c r="K51" s="2">
+        <f t="shared" si="6"/>
+        <v>2.4606121373012009</v>
+      </c>
+      <c r="L51" s="2">
+        <f t="shared" si="7"/>
+        <v>1.6699130656228007</v>
+      </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
@@ -3884,6 +7359,22 @@
       <c r="F52" s="2">
         <v>21.715956857800901</v>
       </c>
+      <c r="H52" s="2">
+        <f t="shared" si="4"/>
+        <v>19.872057633683401</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" si="5"/>
+        <v>3.2853406495058977</v>
+      </c>
+      <c r="K52" s="2">
+        <f t="shared" si="6"/>
+        <v>1.2825079388770995</v>
+      </c>
+      <c r="L52" s="2">
+        <f t="shared" si="7"/>
+        <v>2.0028327106287982</v>
+      </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
@@ -3903,6 +7394,22 @@
       </c>
       <c r="F53" s="2">
         <v>26.7607008278429</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="4"/>
+        <v>24.705846500042099</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" si="5"/>
+        <v>4.1550975078076</v>
+      </c>
+      <c r="K53" s="2">
+        <f t="shared" si="6"/>
+        <v>2.1656962987600998</v>
+      </c>
+      <c r="L53" s="2">
+        <f t="shared" si="7"/>
+        <v>1.9894012090475002</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>